<commit_message>
Added new keywords - China and Chinese
</commit_message>
<xml_diff>
--- a/BiblioPhilly Keywords.xlsx
+++ b/BiblioPhilly Keywords.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotporter/Documents/bibliophilly-keywords-/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet2" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="201">
   <si>
     <t>Book Type</t>
   </si>
@@ -187,6 +203,9 @@
     <t>Carolingian</t>
   </si>
   <si>
+    <t>Chinese</t>
+  </si>
+  <si>
     <t>Christian</t>
   </si>
   <si>
@@ -424,6 +443,9 @@
     <t>Central Asia</t>
   </si>
   <si>
+    <t>China</t>
+  </si>
+  <si>
     <t>Egypt</t>
   </si>
   <si>
@@ -506,6 +528,9 @@
   </si>
   <si>
     <t>Friendship</t>
+  </si>
+  <si>
+    <t>Games</t>
   </si>
   <si>
     <t>Geomancy</t>
@@ -610,24 +635,29 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -636,44 +666,300 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AS7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -783,7 +1069,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -827,7 +1113,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>50</v>
       </c>
@@ -933,358 +1219,367 @@
       <c r="AI3" s="2" t="s">
         <v>84</v>
       </c>
+      <c r="AJ3" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AJ4" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AK4" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AL4" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AM4" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AN4" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AO4" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AP4" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AQ4" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AR4" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AS4" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="AA5" s="2" t="s">
-        <v>156</v>
+      <c r="K6" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="Z6" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="AB6" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="AC6" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7">
+    <row r="7" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new keyword Commentary
</commit_message>
<xml_diff>
--- a/BiblioPhilly Keywords.xlsx
+++ b/BiblioPhilly Keywords.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="206">
   <si>
     <t>Book Type</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Chronicle</t>
+  </si>
+  <si>
+    <t>Commentary</t>
   </si>
   <si>
     <t>Document</t>
@@ -1098,521 +1101,524 @@
       <c r="AL1" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="AM1" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="2" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AJ3" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AK3" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AJ4" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AK4" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AL4" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AM4" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AN4" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AO4" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AP4" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AQ4" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AR4" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AS4" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated keyword list after meeting with Doug, Molly, Jessie
</commit_message>
<xml_diff>
--- a/BiblioPhilly Keywords.xlsx
+++ b/BiblioPhilly Keywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotporter/Documents/bibliophilly-keywords-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65A6E9B7-1DDF-4E49-9EB9-818340EFEBF0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{39AD72A6-2533-D64E-87DA-D3B53CBCBD18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="221">
   <si>
     <t>Book Type</t>
   </si>
@@ -590,6 +590,9 @@
   </si>
   <si>
     <t>Biblical</t>
+  </si>
+  <si>
+    <t>Binding waste</t>
   </si>
   <si>
     <t>Cartography</t>
@@ -696,18 +699,15 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1674,10 +1674,10 @@
         <v>197</v>
       </c>
       <c r="O6" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>199</v>
@@ -1738,11 +1738,14 @@
       </c>
       <c r="AJ6" s="2" t="s">
         <v>218</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with new keywords for Rylands mss
</commit_message>
<xml_diff>
--- a/BiblioPhilly Keywords.xlsx
+++ b/BiblioPhilly Keywords.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dotporter/Documents/bibliophilly-keywords-/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39AD72A6-2533-D64E-87DA-D3B53CBCBD18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet2" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="224">
   <si>
     <t>Book Type</t>
   </si>
@@ -55,6 +46,9 @@
     <t>Commentary</t>
   </si>
   <si>
+    <t>Dictionary</t>
+  </si>
+  <si>
     <t>Document</t>
   </si>
   <si>
@@ -145,6 +139,9 @@
     <t>Scribal manual</t>
   </si>
   <si>
+    <t>Song book</t>
+  </si>
+  <si>
     <t>Torah</t>
   </si>
   <si>
@@ -569,6 +566,9 @@
   </si>
   <si>
     <t>Turkey</t>
+  </si>
+  <si>
+    <t>Wales</t>
   </si>
   <si>
     <t>Yemen</t>
@@ -688,24 +688,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="4">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
     </font>
+    <font/>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -715,7 +710,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -725,350 +720,53 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BC8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="16.14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1126,10 +824,10 @@
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="2" t="s">
@@ -1198,557 +896,566 @@
       <c r="AQ1" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="AR1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AJ3" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AK3" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AL3" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="AM3" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4">
       <c r="A4" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AJ4" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="AK4" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AL4" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AM4" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AN4" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AO4" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AP4" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AQ4" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AR4" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AS4" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AT4" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AU4" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AV4" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AW4" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AX4" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AY4" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AZ4" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="BA4" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="BB4" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="BC4" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5">
       <c r="A5" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="AA5" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>183</v>
+      <c r="Q6" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="AG6" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="AI6" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="AK6" s="2" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="6" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="Z6" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="AB6" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="AC6" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="AE6" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="AF6" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="AG6" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="AH6" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="AI6" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="AJ6" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="AK6" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8">
       <c r="B8" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>